<commit_message>
Modificación CU 15 - Consultar grupos y rentas
Se establece una vista de horario incluyendo rentas y grupos para el CU
15 - consultar grupos y rentas, y se modificac el CU 12 - CRU Grupo
permitiendo agregar varios días.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="107">
   <si>
     <t>Columna</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Por iniciar</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -578,12 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -613,6 +610,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,7 +926,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,84 +1001,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="22"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="22"/>
+      <c r="L4" s="35"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="22"/>
+      <c r="O4" s="35"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="22"/>
+      <c r="R4" s="35"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="21" t="s">
+      <c r="T4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="22"/>
+      <c r="U4" s="35"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="22"/>
+      <c r="X4" s="35"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="21" t="s">
+      <c r="Z4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="22"/>
+      <c r="AA4" s="35"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="21" t="s">
+      <c r="AC4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="22"/>
+      <c r="AD4" s="35"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="21" t="s">
+      <c r="AF4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="22"/>
+      <c r="AG4" s="35"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="21" t="s">
+      <c r="AI4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="22"/>
+      <c r="AJ4" s="35"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="21" t="s">
+      <c r="AL4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="22"/>
+      <c r="AM4" s="35"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="21" t="s">
+      <c r="AO4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="22"/>
+      <c r="AP4" s="35"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="21" t="s">
+      <c r="AR4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="22"/>
+      <c r="AS4" s="35"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="21" t="s">
+      <c r="AU4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="22"/>
+      <c r="AV4" s="35"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="21" t="s">
+      <c r="AX4" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="22"/>
-      <c r="AZ4" s="21" t="s">
+      <c r="AY4" s="35"/>
+      <c r="AZ4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="22"/>
+      <c r="BA4" s="35"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1208,21 +1211,25 @@
       </c>
     </row>
     <row r="6" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8"/>
+        <v>106</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2</v>
+      </c>
       <c r="I6" s="8">
         <f>G6-H6</f>
         <v>0</v>
@@ -1313,7 +1320,7 @@
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA17" si="15">G6-AZ6</f>
@@ -1321,12 +1328,12 @@
       </c>
     </row>
     <row r="7" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="29" t="s">
         <v>76</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1432,12 +1439,12 @@
       </c>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="30" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1543,12 +1550,12 @@
       </c>
     </row>
     <row r="9" spans="2:53" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1654,12 +1661,12 @@
       </c>
     </row>
     <row r="10" spans="2:53" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1765,12 +1772,12 @@
       </c>
     </row>
     <row r="11" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="30" t="s">
         <v>77</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1876,12 +1883,12 @@
       </c>
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="32" t="s">
         <v>78</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1987,12 +1994,12 @@
       </c>
     </row>
     <row r="13" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -2098,12 +2105,12 @@
       </c>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="33" t="s">
         <v>77</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2209,14 +2216,14 @@
       </c>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="22" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="33" t="s">
         <v>77</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2322,12 +2329,12 @@
       </c>
     </row>
     <row r="16" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -2433,14 +2440,14 @@
       </c>
     </row>
     <row r="17" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -2546,14 +2553,14 @@
       </c>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -2659,14 +2666,14 @@
       </c>
     </row>
     <row r="19" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -2772,14 +2779,14 @@
       </c>
     </row>
     <row r="20" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -2885,14 +2892,14 @@
       </c>
     </row>
     <row r="21" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -2998,14 +3005,14 @@
       </c>
     </row>
     <row r="22" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -3111,14 +3118,14 @@
       </c>
     </row>
     <row r="23" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="22" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -3224,14 +3231,14 @@
       </c>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -3337,14 +3344,14 @@
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="22" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -3450,14 +3457,14 @@
       </c>
     </row>
     <row r="26" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -3563,14 +3570,14 @@
       </c>
     </row>
     <row r="27" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -3676,14 +3683,14 @@
       </c>
     </row>
     <row r="28" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -3789,14 +3796,14 @@
       </c>
     </row>
     <row r="29" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -3902,14 +3909,14 @@
       </c>
     </row>
     <row r="30" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -4015,14 +4022,14 @@
       </c>
     </row>
     <row r="31" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="22" t="s">
         <v>56</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -4128,14 +4135,14 @@
       </c>
     </row>
     <row r="32" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="22" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -4241,14 +4248,14 @@
       </c>
     </row>
     <row r="33" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="22" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="5" t="s">
@@ -4354,14 +4361,14 @@
       </c>
     </row>
     <row r="34" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="22" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -4467,14 +4474,14 @@
       </c>
     </row>
     <row r="35" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="22" t="s">
         <v>60</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -4580,14 +4587,14 @@
       </c>
     </row>
     <row r="36" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="22" t="s">
         <v>61</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -4693,14 +4700,14 @@
       </c>
     </row>
     <row r="37" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="22" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -4806,14 +4813,14 @@
       </c>
     </row>
     <row r="38" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="22" t="s">
         <v>63</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E38" s="34" t="s">
+      <c r="E38" s="32" t="s">
         <v>75</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -4919,14 +4926,14 @@
       </c>
     </row>
     <row r="39" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="27" t="s">
+      <c r="D39" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="33" t="s">
+      <c r="E39" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -5032,14 +5039,14 @@
       </c>
     </row>
     <row r="40" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C40" s="13"/>
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E40" s="33" t="s">
+      <c r="E40" s="31" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -5254,11 +5261,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5270,6 +5272,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Descripciones de CU 23 y 24, modificacion de mockups
Se agregan las descripciones de los casos de uso Buscar profesor y buscar cliente, se editan los mockups de los casos de uso CRU profesor, CRU alumno
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -919,14 +919,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,8 +1339,12 @@
       <c r="F7" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" ref="I7:I17" si="16">G7-H7</f>
         <v>0</v>
@@ -1431,7 +1435,7 @@
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
@@ -5261,6 +5265,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5272,11 +5281,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5294,7 +5298,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Segunda parte de la redacción
Segunda parte de la redacción de la especificación de requierimientos,
se actualiza la lista de tareas para la segunda iteración y se cambia en
el modelo de casos de uso el CU 11 - Cmabiar alumno de grupo, pasando de
director a profesor.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -919,14 +919,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1337,7 @@
         <v>76</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1452,16 +1452,20 @@
         <v>77</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="8"/>
+      <c r="K8" s="8">
+        <v>1</v>
+      </c>
       <c r="L8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1546,7 +1550,7 @@
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
@@ -1565,103 +1569,107 @@
       <c r="F9" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="8"/>
+      <c r="K9" s="8">
+        <v>2</v>
+      </c>
       <c r="L9" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="8"/>
       <c r="AG9" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH9" s="10"/>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK9" s="10"/>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN9" s="10"/>
       <c r="AO9" s="8"/>
       <c r="AP9" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT9" s="10"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW9" s="10"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ9" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="2:53" ht="60" x14ac:dyDescent="0.25">
@@ -1676,103 +1684,107 @@
       <c r="F10" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="8"/>
+      <c r="K10" s="8">
+        <v>2</v>
+      </c>
       <c r="L10" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="2:53" x14ac:dyDescent="0.25">
@@ -1787,14 +1799,18 @@
       <c r="F11" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8">
         <f t="shared" ref="I11" si="17">G11-H11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
       <c r="L11" s="8">
         <f t="shared" ref="L11" si="18">I11-K11</f>
         <v>0</v>
@@ -1879,7 +1895,7 @@
       </c>
       <c r="AZ11" s="11">
         <f t="shared" ref="AZ11" si="32">H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA11" s="11">
         <f t="shared" ref="BA11" si="33">G11-AZ11</f>
@@ -5298,7 +5314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
CU 25 - Consultar gastos
Se agrega el CU 25 - Consultar gastos, se modificacn los prototipos de
los CU 16 y 17, se actualikza la lista de tareas, se actualiza la
especificación de requerimientos.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -923,10 +923,10 @@
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,105 +2027,109 @@
         <v>76</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M13" s="10"/>
-      <c r="N13" s="8"/>
+      <c r="N13" s="8">
+        <v>3</v>
+      </c>
       <c r="O13" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S13" s="10"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.25">
@@ -2138,22 +2142,26 @@
         <v>77</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="10"/>
-      <c r="N14" s="8"/>
+      <c r="N14" s="8">
+        <v>1</v>
+      </c>
       <c r="O14" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2232,7 +2240,7 @@
       </c>
       <c r="AZ14" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA14" s="11">
         <f t="shared" si="15"/>
@@ -5285,6 +5293,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5296,11 +5309,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 01 y 02
Diagramas de robustez y secuencia de los CU 01 - CRU Promoción y 02 -
Registrar pago de alumno, se actualiza la lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -923,10 +923,10 @@
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,28 +2259,32 @@
         <v>77</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" s="10"/>
-      <c r="Q15" s="8"/>
+      <c r="Q15" s="8">
+        <v>1</v>
+      </c>
       <c r="R15" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2353,7 +2357,7 @@
       </c>
       <c r="AZ15" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA15" s="11">
         <f t="shared" si="15"/>
@@ -2370,105 +2374,109 @@
         <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" s="10"/>
-      <c r="Q16" s="8"/>
+      <c r="Q16" s="8">
+        <v>3</v>
+      </c>
       <c r="R16" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S16" s="10"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V16" s="10"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y16" s="10"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB16" s="10"/>
       <c r="AC16" s="8"/>
       <c r="AD16" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE16" s="10"/>
       <c r="AF16" s="8"/>
       <c r="AG16" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH16" s="10"/>
       <c r="AI16" s="8"/>
       <c r="AJ16" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK16" s="10"/>
       <c r="AL16" s="8"/>
       <c r="AM16" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN16" s="10"/>
       <c r="AO16" s="8"/>
       <c r="AP16" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="8"/>
       <c r="AS16" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT16" s="10"/>
       <c r="AU16" s="8"/>
       <c r="AV16" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW16" s="10"/>
       <c r="AX16" s="8"/>
       <c r="AY16" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ16" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA16" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="2:53" x14ac:dyDescent="0.25">
@@ -2483,34 +2491,38 @@
         <v>75</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="10"/>
-      <c r="T17" s="8"/>
+      <c r="T17" s="8">
+        <v>1</v>
+      </c>
       <c r="U17" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2577,7 +2589,7 @@
       </c>
       <c r="AZ17" s="11">
         <f>H17+K17+N17+Q17+T17+W17+Z17+AC17+AF17+AI17+AL17+AO17+AR17+AU17+AX17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="11">
         <f t="shared" si="15"/>
@@ -2596,34 +2608,38 @@
         <v>75</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8">
         <f t="shared" ref="I18:I40" si="34">G18-H18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8">
         <f t="shared" ref="L18:L40" si="35">I18-K18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8">
         <f t="shared" ref="O18:O40" si="36">L18-N18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8">
         <f t="shared" ref="R18:R40" si="37">O18-Q18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="10"/>
-      <c r="T18" s="8"/>
+      <c r="T18" s="8">
+        <v>1</v>
+      </c>
       <c r="U18" s="8">
         <f t="shared" ref="U18:U40" si="38">R18-T18</f>
         <v>0</v>
@@ -2690,7 +2706,7 @@
       </c>
       <c r="AZ18" s="11">
         <f>H18+K18+N18+Q18+T18+W18+Z18+AC18+AF18+AI18+AL18+AO18+AR18+AU18+AX18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="11">
         <f t="shared" ref="BA18:BA40" si="49">G18-AZ18</f>
@@ -2709,34 +2725,38 @@
         <v>76</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8">
         <f>G19-H19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="10"/>
-      <c r="T19" s="8"/>
+      <c r="T19" s="8">
+        <v>1</v>
+      </c>
       <c r="U19" s="8">
         <f t="shared" si="38"/>
         <v>0</v>
@@ -2803,7 +2823,7 @@
       </c>
       <c r="AZ19" s="11">
         <f t="shared" ref="AZ19:AZ29" si="50">H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA19" s="11">
         <f t="shared" si="49"/>
@@ -2822,34 +2842,38 @@
         <v>76</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8">
         <f t="shared" ref="I20:I31" si="51">G20-H20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="10"/>
-      <c r="T20" s="8"/>
+      <c r="T20" s="8">
+        <v>1</v>
+      </c>
       <c r="U20" s="8">
         <f t="shared" si="38"/>
         <v>0</v>
@@ -2916,7 +2940,7 @@
       </c>
       <c r="AZ20" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA20" s="11">
         <f t="shared" si="49"/>
@@ -5293,11 +5317,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5309,6 +5328,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 05 y 07.
Se agregan los diagramas de robustez y secuencia de los CU 05 -
Registrar asistencia y 07 - Consultar grupos, se modifica la discripción
del CU 07 - Consultar grupos, se actualiza el modelo de dominio y se
actualizan las plantillas de casos de uso y lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -926,7 +926,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,40 +2959,44 @@
         <v>75</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="10"/>
-      <c r="W21" s="8"/>
+      <c r="W21" s="8">
+        <v>1</v>
+      </c>
       <c r="X21" s="8">
         <f t="shared" si="39"/>
         <v>0</v>
@@ -3053,7 +3057,7 @@
       </c>
       <c r="AZ21" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA21" s="11">
         <f t="shared" si="49"/>
@@ -3072,40 +3076,44 @@
         <v>75</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="10"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22" s="10"/>
-      <c r="W22" s="8"/>
+      <c r="W22" s="8">
+        <v>1</v>
+      </c>
       <c r="X22" s="8">
         <f t="shared" si="39"/>
         <v>0</v>
@@ -3166,7 +3174,7 @@
       </c>
       <c r="AZ22" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA22" s="11">
         <f t="shared" si="49"/>
@@ -3187,95 +3195,97 @@
       <c r="F23" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="10"/>
       <c r="W23" s="8"/>
       <c r="X23" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="8"/>
       <c r="AA23" s="8">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23" s="10"/>
       <c r="AF23" s="8"/>
       <c r="AG23" s="8">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH23" s="10"/>
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK23" s="10"/>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN23" s="10"/>
       <c r="AO23" s="8"/>
       <c r="AP23" s="8">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="8"/>
       <c r="AS23" s="8">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT23" s="10"/>
       <c r="AU23" s="8"/>
       <c r="AV23" s="8">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW23" s="10"/>
       <c r="AX23" s="8"/>
       <c r="AY23" s="8">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ23" s="11">
         <f t="shared" si="50"/>
@@ -3283,7 +3293,7 @@
       </c>
       <c r="BA23" s="11">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.25">
@@ -3300,95 +3310,97 @@
       <c r="F24" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE24" s="10"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH24" s="10"/>
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK24" s="10"/>
       <c r="AL24" s="8"/>
       <c r="AM24" s="8">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN24" s="10"/>
       <c r="AO24" s="8"/>
       <c r="AP24" s="8">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ24" s="10"/>
       <c r="AR24" s="8"/>
       <c r="AS24" s="8">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT24" s="10"/>
       <c r="AU24" s="8"/>
       <c r="AV24" s="8">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW24" s="10"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ24" s="11">
         <f t="shared" si="50"/>
@@ -3396,7 +3408,7 @@
       </c>
       <c r="BA24" s="11">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
@@ -5317,6 +5329,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5328,11 +5345,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 22 y 8
Se realizan los diagramas de robustez y secuencia de los casos de uso iniciar sesion e inscribir alumno asi como modificaciones menores en las descripciones de estos.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,8 +620,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -919,14 +947,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3228,72 +3256,74 @@
         <v>1</v>
       </c>
       <c r="V23" s="10"/>
-      <c r="W23" s="8"/>
+      <c r="W23" s="8">
+        <v>1</v>
+      </c>
       <c r="X23" s="8">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="8"/>
       <c r="AA23" s="8">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE23" s="10"/>
       <c r="AF23" s="8"/>
       <c r="AG23" s="8">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH23" s="10"/>
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK23" s="10"/>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN23" s="10"/>
       <c r="AO23" s="8"/>
       <c r="AP23" s="8">
         <f t="shared" si="45"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="8"/>
       <c r="AS23" s="8">
         <f t="shared" si="46"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT23" s="10"/>
       <c r="AU23" s="8"/>
       <c r="AV23" s="8">
         <f t="shared" si="47"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW23" s="10"/>
       <c r="AX23" s="8"/>
       <c r="AY23" s="8">
         <f t="shared" si="48"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ23" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA23" s="11">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.25">
@@ -3343,72 +3373,74 @@
         <v>1</v>
       </c>
       <c r="V24" s="10"/>
-      <c r="W24" s="8"/>
+      <c r="W24" s="8">
+        <v>1</v>
+      </c>
       <c r="X24" s="8">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE24" s="10"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH24" s="10"/>
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK24" s="10"/>
       <c r="AL24" s="8"/>
       <c r="AM24" s="8">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN24" s="10"/>
       <c r="AO24" s="8"/>
       <c r="AP24" s="8">
         <f t="shared" si="45"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ24" s="10"/>
       <c r="AR24" s="8"/>
       <c r="AS24" s="8">
         <f t="shared" si="46"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT24" s="10"/>
       <c r="AU24" s="8"/>
       <c r="AV24" s="8">
         <f t="shared" si="47"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW24" s="10"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8">
         <f t="shared" si="48"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ24" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA24" s="11">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
@@ -5329,11 +5361,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5345,6 +5372,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5362,7 +5394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 10 y 11
Diagramas de robustez y secuencia de los CU 10 - CRU Alumno y 11 -
Cambiar alumno de grupo, se hacen modificaciones menores a los diagramas
de los CU 07 y 08, se le quitan flujos alternos al CU 11, se agregan
métodos al modelo de dominio y se actualizan las plantillas de casos de
uso y tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +645,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -947,14 +947,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W23" sqref="W23"/>
+      <selection pane="bottomRight" activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,7 +3221,7 @@
         <v>76</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G23" s="5">
         <v>1</v>
@@ -3338,7 +3338,7 @@
         <v>76</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G24" s="5">
         <v>1</v>
@@ -3455,46 +3455,50 @@
         <v>75</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="10"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" s="10"/>
       <c r="W25" s="8"/>
       <c r="X25" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y25" s="10"/>
-      <c r="Z25" s="8"/>
+      <c r="Z25" s="8">
+        <v>1</v>
+      </c>
       <c r="AA25" s="8">
         <f t="shared" si="40"/>
         <v>0</v>
@@ -3549,7 +3553,7 @@
       </c>
       <c r="AZ25" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA25" s="11">
         <f t="shared" si="49"/>
@@ -3568,46 +3572,50 @@
         <v>75</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="10"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="10"/>
       <c r="W26" s="8"/>
       <c r="X26" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y26" s="10"/>
-      <c r="Z26" s="8"/>
+      <c r="Z26" s="8">
+        <v>1</v>
+      </c>
       <c r="AA26" s="8">
         <f t="shared" si="40"/>
         <v>0</v>
@@ -3662,7 +3670,7 @@
       </c>
       <c r="AZ26" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA26" s="11">
         <f t="shared" si="49"/>
@@ -3681,46 +3689,50 @@
         <v>76</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27" s="10"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V27" s="10"/>
       <c r="W27" s="8"/>
       <c r="X27" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y27" s="10"/>
-      <c r="Z27" s="8"/>
+      <c r="Z27" s="8">
+        <v>1</v>
+      </c>
       <c r="AA27" s="8">
         <f t="shared" si="40"/>
         <v>0</v>
@@ -3775,7 +3787,7 @@
       </c>
       <c r="AZ27" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA27" s="11">
         <f t="shared" si="49"/>
@@ -3794,46 +3806,50 @@
         <v>76</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
       <c r="H28" s="8"/>
       <c r="I28" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28" s="10"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="10"/>
       <c r="W28" s="8"/>
       <c r="X28" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y28" s="10"/>
-      <c r="Z28" s="8"/>
+      <c r="Z28" s="8">
+        <v>1</v>
+      </c>
       <c r="AA28" s="8">
         <f t="shared" si="40"/>
         <v>0</v>
@@ -3888,7 +3904,7 @@
       </c>
       <c r="AZ28" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA28" s="11">
         <f t="shared" si="49"/>
@@ -5394,7 +5410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 12 y 15
Diagramas de robustez y secuencia de los CU 12 - CRU Grupo y 15 -
Consultar grupos y rentas, se modifican las descripciones de los CU 12 y
15, se agregan métodos al modelo de dominio y se actualizan las
plantillas de casos de uso y tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -951,10 +951,10 @@
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="M18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z28" sqref="Z28"/>
+      <selection pane="bottomRight" activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3923,52 +3923,56 @@
         <v>75</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
       <c r="H29" s="8"/>
       <c r="I29" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="8"/>
       <c r="O29" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29" s="10"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V29" s="10"/>
       <c r="W29" s="8"/>
       <c r="X29" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y29" s="10"/>
       <c r="Z29" s="8"/>
       <c r="AA29" s="8">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB29" s="10"/>
-      <c r="AC29" s="8"/>
+      <c r="AC29" s="8">
+        <v>1</v>
+      </c>
       <c r="AD29" s="8">
         <f t="shared" si="41"/>
         <v>0</v>
@@ -4017,7 +4021,7 @@
       </c>
       <c r="AZ29" s="11">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA29" s="11">
         <f t="shared" si="49"/>
@@ -4036,52 +4040,56 @@
         <v>75</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30" s="10"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30" s="10"/>
       <c r="W30" s="8"/>
       <c r="X30" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y30" s="10"/>
       <c r="Z30" s="8"/>
       <c r="AA30" s="8">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB30" s="10"/>
-      <c r="AC30" s="8"/>
+      <c r="AC30" s="8">
+        <v>1</v>
+      </c>
       <c r="AD30" s="8">
         <f t="shared" si="41"/>
         <v>0</v>
@@ -4130,7 +4138,7 @@
       </c>
       <c r="AZ30" s="11">
         <f>H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA30" s="11">
         <f t="shared" si="49"/>

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU13 y 14
Se crean los diagramas de robustez y secuencia de los casos de uso
Consultar historial de pago de profesores y registrar pago de profesor
asi como modificaciones menores en el modelo de dominio
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -356,7 +351,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +640,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -947,14 +942,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="M18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AB33" sqref="AB33"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4157,52 +4152,56 @@
         <v>76</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8">
         <f t="shared" ref="L31:L38" si="52">I31-K31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8">
         <f t="shared" ref="O31:O38" si="53">L31-N31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8">
         <f t="shared" ref="R31:R38" si="54">O31-Q31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S31" s="10"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8">
         <f t="shared" ref="U31:U38" si="55">R31-T31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V31" s="10"/>
       <c r="W31" s="8"/>
       <c r="X31" s="8">
         <f t="shared" ref="X31:X38" si="56">U31-W31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y31" s="10"/>
       <c r="Z31" s="8"/>
       <c r="AA31" s="8">
         <f t="shared" ref="AA31:AA38" si="57">X31-Z31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB31" s="10"/>
-      <c r="AC31" s="8"/>
+      <c r="AC31" s="8">
+        <v>1</v>
+      </c>
       <c r="AD31" s="8">
         <f t="shared" ref="AD31:AD38" si="58">AA31-AC31</f>
         <v>0</v>
@@ -4251,7 +4250,7 @@
       </c>
       <c r="AZ31" s="11">
         <f>H31+K31+N31+Q31+T31+W31+Z31+AC31+AF31+AI31+AL31+AO31+AR31+AU31+AX31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA31" s="11">
         <f t="shared" ref="BA31:BA38" si="66">G31-AZ31</f>
@@ -4270,52 +4269,56 @@
         <v>76</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8">
         <f t="shared" ref="I32:I39" si="67">G32-H32</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S32" s="10"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32" s="10"/>
       <c r="W32" s="8"/>
       <c r="X32" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y32" s="10"/>
       <c r="Z32" s="8"/>
       <c r="AA32" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB32" s="10"/>
-      <c r="AC32" s="8"/>
+      <c r="AC32" s="8">
+        <v>1</v>
+      </c>
       <c r="AD32" s="8">
         <f t="shared" si="58"/>
         <v>0</v>
@@ -4364,7 +4367,7 @@
       </c>
       <c r="AZ32" s="11">
         <f t="shared" ref="AZ32:AZ37" si="68">H32+K32+N32+Q32+T32+W32+Z32+AC32+AF32+AI32+AL32+AO32+AR32+AU32+AX32</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA32" s="11">
         <f t="shared" si="66"/>
@@ -5385,6 +5388,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5396,11 +5404,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5418,7 +5421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 18 y 19
Diagramas de robustez y secuencia de los CU 18 - Generar reporte de
ingresos y egresos y 19 - CRU Renta de espacio, se modificacn las
descripciones de los CU 18 y 19, se agregan métodos al modelo de
dominio, se actualizan las plantillas de casos de uso y lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -351,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -640,7 +645,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -699,7 +704,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -732,9 +737,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -767,6 +789,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -942,14 +981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AB24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="AF36" sqref="AF36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,58 +4425,62 @@
         <v>75</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33" s="10"/>
       <c r="T33" s="8"/>
       <c r="U33" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33" s="10"/>
       <c r="W33" s="8"/>
       <c r="X33" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y33" s="10"/>
       <c r="Z33" s="8"/>
       <c r="AA33" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB33" s="10"/>
       <c r="AC33" s="8"/>
       <c r="AD33" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE33" s="10"/>
-      <c r="AF33" s="8"/>
+      <c r="AF33" s="8">
+        <v>1</v>
+      </c>
       <c r="AG33" s="8">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -4480,7 +4523,7 @@
       </c>
       <c r="AZ33" s="11">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA33" s="11">
         <f t="shared" si="66"/>
@@ -4499,58 +4542,62 @@
         <v>75</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G34" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S34" s="10"/>
       <c r="T34" s="8"/>
       <c r="U34" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V34" s="10"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y34" s="10"/>
       <c r="Z34" s="8"/>
       <c r="AA34" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB34" s="10"/>
       <c r="AC34" s="8"/>
       <c r="AD34" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34" s="10"/>
-      <c r="AF34" s="8"/>
+      <c r="AF34" s="8">
+        <v>1</v>
+      </c>
       <c r="AG34" s="8">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -4593,7 +4640,7 @@
       </c>
       <c r="AZ34" s="11">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA34" s="11">
         <f t="shared" si="66"/>
@@ -5421,7 +5468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 16 y 17
Se crean los diagramas de robustez y secuencia de los casos de uso CRU egreso CRU gasto promocional asi como correcciones en las descripciones de casos de uso
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +645,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -981,14 +981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AB24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="S21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF36" sqref="AF36"/>
+      <selection pane="bottomRight" activeCell="AF37" sqref="AF37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4659,58 +4659,62 @@
         <v>76</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
       <c r="H35" s="8"/>
       <c r="I35" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="10"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S35" s="10"/>
       <c r="T35" s="8"/>
       <c r="U35" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V35" s="10"/>
       <c r="W35" s="8"/>
       <c r="X35" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y35" s="10"/>
       <c r="Z35" s="8"/>
       <c r="AA35" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB35" s="10"/>
       <c r="AC35" s="8"/>
       <c r="AD35" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE35" s="10"/>
-      <c r="AF35" s="8"/>
+      <c r="AF35" s="8">
+        <v>1</v>
+      </c>
       <c r="AG35" s="8">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -4753,7 +4757,7 @@
       </c>
       <c r="AZ35" s="11">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA35" s="11">
         <f t="shared" si="66"/>
@@ -4772,58 +4776,62 @@
         <v>76</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G36" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
       <c r="H36" s="8"/>
       <c r="I36" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="10"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="10"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S36" s="10"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V36" s="10"/>
       <c r="W36" s="8"/>
       <c r="X36" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y36" s="10"/>
       <c r="Z36" s="8"/>
       <c r="AA36" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB36" s="10"/>
       <c r="AC36" s="8"/>
       <c r="AD36" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE36" s="10"/>
-      <c r="AF36" s="8"/>
+      <c r="AF36" s="8">
+        <v>1</v>
+      </c>
       <c r="AG36" s="8">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -4866,7 +4874,7 @@
       </c>
       <c r="AZ36" s="11">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA36" s="11">
         <f t="shared" si="66"/>
@@ -5435,11 +5443,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5451,6 +5454,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5468,7 +5476,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia de casos de uso 23 y 24
Se crean los diagramas de robustez y secuencia de los casos de uso consultar profesores y consultar clientes asi como modificaciones menores en la dscripcion de ambos
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -985,10 +985,10 @@
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="S21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="V30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF37" sqref="AF37"/>
+      <selection pane="bottomRight" activeCell="AI39" sqref="AI39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5119,64 +5119,68 @@
         <v>76</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G39" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="10"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8">
         <f t="shared" ref="L39" si="69">I39-K39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="10"/>
       <c r="N39" s="8"/>
       <c r="O39" s="8">
         <f t="shared" ref="O39" si="70">L39-N39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P39" s="10"/>
       <c r="Q39" s="8"/>
       <c r="R39" s="8">
         <f t="shared" ref="R39" si="71">O39-Q39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S39" s="10"/>
       <c r="T39" s="8"/>
       <c r="U39" s="8">
         <f t="shared" ref="U39" si="72">R39-T39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V39" s="10"/>
       <c r="W39" s="8"/>
       <c r="X39" s="8">
         <f t="shared" ref="X39" si="73">U39-W39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y39" s="10"/>
       <c r="Z39" s="8"/>
       <c r="AA39" s="8">
         <f t="shared" ref="AA39" si="74">X39-Z39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB39" s="10"/>
       <c r="AC39" s="8"/>
       <c r="AD39" s="8">
         <f t="shared" ref="AD39" si="75">AA39-AC39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE39" s="10"/>
       <c r="AF39" s="8"/>
       <c r="AG39" s="8">
         <f t="shared" ref="AG39" si="76">AD39-AF39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH39" s="10"/>
-      <c r="AI39" s="8"/>
+      <c r="AI39" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ39" s="8">
         <f t="shared" ref="AJ39" si="77">AG39-AI39</f>
         <v>0</v>
@@ -5213,7 +5217,7 @@
       </c>
       <c r="AZ39" s="11">
         <f>H39+K39+N39+Q39+T39+W39+Z39+AC39+AF39+AI39+AL39+AO39+AR39+AU39+AX39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA39" s="11">
         <f t="shared" ref="BA39" si="83">G39-AZ39</f>
@@ -5232,64 +5236,68 @@
         <v>76</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G40" s="13"/>
+        <v>106</v>
+      </c>
+      <c r="G40" s="13">
+        <v>1</v>
+      </c>
       <c r="H40" s="14"/>
       <c r="I40" s="14">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="15"/>
       <c r="K40" s="14"/>
       <c r="L40" s="14">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="15"/>
       <c r="N40" s="14"/>
       <c r="O40" s="14">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P40" s="15"/>
       <c r="Q40" s="14"/>
       <c r="R40" s="14">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S40" s="15"/>
       <c r="T40" s="14"/>
       <c r="U40" s="14">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V40" s="15"/>
       <c r="W40" s="14"/>
       <c r="X40" s="14">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y40" s="15"/>
       <c r="Z40" s="14"/>
       <c r="AA40" s="14">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB40" s="15"/>
       <c r="AC40" s="14"/>
       <c r="AD40" s="14">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE40" s="15"/>
       <c r="AF40" s="14"/>
       <c r="AG40" s="14">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH40" s="15"/>
-      <c r="AI40" s="14"/>
+      <c r="AI40" s="14">
+        <v>1</v>
+      </c>
       <c r="AJ40" s="14">
         <f t="shared" si="43"/>
         <v>0</v>
@@ -5443,6 +5451,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5454,11 +5467,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 20 y 21
Diagramas de robustez y secuencia de CU 20 - CRU Profesor y 21 - CRU
Cliente, se modifican sus respectivas descripciones y se actualizan las
plantillas de casos de uso y lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
   <si>
     <t>Columna</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>Realizar diagramas de robustez y secuencia de CU 24.</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>Hecho</t>
@@ -356,7 +353,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +642,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -981,14 +978,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="V30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AJ6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI39" sqref="AI39"/>
+      <selection pane="bottomRight" activeCell="AG38" sqref="AG38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1281,7 @@
         <v>75</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="5">
         <v>2</v>
@@ -1399,7 +1396,7 @@
         <v>76</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1514,7 +1511,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1629,7 +1626,7 @@
         <v>76</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
@@ -1744,7 +1741,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -1859,7 +1856,7 @@
         <v>77</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1974,7 +1971,7 @@
         <v>78</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
@@ -2089,7 +2086,7 @@
         <v>76</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="5">
         <v>2</v>
@@ -2204,7 +2201,7 @@
         <v>77</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="5">
         <v>1</v>
@@ -2321,7 +2318,7 @@
         <v>77</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="5">
         <v>1</v>
@@ -2436,7 +2433,7 @@
         <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="5">
         <v>2</v>
@@ -2553,7 +2550,7 @@
         <v>75</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="5">
         <v>1</v>
@@ -2670,7 +2667,7 @@
         <v>75</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="5">
         <v>1</v>
@@ -2787,7 +2784,7 @@
         <v>76</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="5">
         <v>1</v>
@@ -2904,7 +2901,7 @@
         <v>76</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="5">
         <v>1</v>
@@ -3021,7 +3018,7 @@
         <v>75</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="5">
         <v>1</v>
@@ -3138,7 +3135,7 @@
         <v>75</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="5">
         <v>1</v>
@@ -3255,7 +3252,7 @@
         <v>76</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" s="5">
         <v>1</v>
@@ -3372,7 +3369,7 @@
         <v>76</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G24" s="5">
         <v>1</v>
@@ -3489,7 +3486,7 @@
         <v>75</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" s="5">
         <v>1</v>
@@ -3606,7 +3603,7 @@
         <v>75</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -3723,7 +3720,7 @@
         <v>76</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G27" s="5">
         <v>1</v>
@@ -3840,7 +3837,7 @@
         <v>76</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G28" s="5">
         <v>1</v>
@@ -3957,7 +3954,7 @@
         <v>75</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G29" s="5">
         <v>1</v>
@@ -4074,7 +4071,7 @@
         <v>75</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G30" s="5">
         <v>1</v>
@@ -4191,7 +4188,7 @@
         <v>76</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G31" s="5">
         <v>1</v>
@@ -4308,7 +4305,7 @@
         <v>76</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G32" s="5">
         <v>1</v>
@@ -4425,7 +4422,7 @@
         <v>75</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G33" s="5">
         <v>1</v>
@@ -4542,7 +4539,7 @@
         <v>75</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G34" s="5">
         <v>1</v>
@@ -4659,7 +4656,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G35" s="5">
         <v>1</v>
@@ -4776,7 +4773,7 @@
         <v>76</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G36" s="5">
         <v>1</v>
@@ -4895,103 +4892,107 @@
       <c r="F37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
       <c r="H37" s="8"/>
       <c r="I37" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="10"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S37" s="10"/>
       <c r="T37" s="8"/>
       <c r="U37" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V37" s="10"/>
       <c r="W37" s="8"/>
       <c r="X37" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y37" s="10"/>
       <c r="Z37" s="8"/>
       <c r="AA37" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB37" s="10"/>
       <c r="AC37" s="8"/>
       <c r="AD37" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE37" s="10"/>
       <c r="AF37" s="8"/>
       <c r="AG37" s="8">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH37" s="10"/>
-      <c r="AI37" s="8"/>
+      <c r="AI37" s="8">
+        <v>2</v>
+      </c>
       <c r="AJ37" s="8">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK37" s="10"/>
       <c r="AL37" s="8"/>
       <c r="AM37" s="8">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN37" s="10"/>
       <c r="AO37" s="8"/>
       <c r="AP37" s="8">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ37" s="10"/>
       <c r="AR37" s="8"/>
       <c r="AS37" s="8">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT37" s="10"/>
       <c r="AU37" s="8"/>
       <c r="AV37" s="8">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW37" s="10"/>
       <c r="AX37" s="8"/>
       <c r="AY37" s="8">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ37" s="11">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA37" s="11">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38" spans="2:53" x14ac:dyDescent="0.25">
@@ -5008,62 +5009,66 @@
       <c r="F38" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="5"/>
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="10"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="10"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38" s="10"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S38" s="10"/>
       <c r="T38" s="8"/>
       <c r="U38" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V38" s="10"/>
       <c r="W38" s="8"/>
       <c r="X38" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y38" s="10"/>
       <c r="Z38" s="8"/>
       <c r="AA38" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB38" s="10"/>
       <c r="AC38" s="8"/>
       <c r="AD38" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE38" s="10"/>
       <c r="AF38" s="8"/>
       <c r="AG38" s="8">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH38" s="10"/>
-      <c r="AI38" s="8"/>
+      <c r="AI38" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ38" s="8">
         <f t="shared" si="60"/>
         <v>0</v>
@@ -5100,7 +5105,7 @@
       </c>
       <c r="AZ38" s="11">
         <f>H38+K38+N38+Q38+T38+W38+Z38+AC38+AF38+AI38+AL38+AO38+AR38+AU38+AX38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA38" s="11">
         <f t="shared" si="66"/>
@@ -5119,7 +5124,7 @@
         <v>76</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G39" s="5">
         <v>1</v>
@@ -5236,7 +5241,7 @@
         <v>76</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G40" s="13">
         <v>1</v>
@@ -5451,11 +5456,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -5467,6 +5467,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5484,7 +5489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Descripción de caso de uso 26, diagrama de robustez, secuencia y correcciones menores.
Se crea el diagrama de robustez, secuencia, descripción de caso de uso y mockup del caso de usomodificar cuenta de usuario, asi como correcciones  menores.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 2da Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
   <si>
     <t>Columna</t>
   </si>
@@ -348,12 +348,27 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>CU 25</t>
+  </si>
+  <si>
+    <t>Realizar diagramas de robustez y secuencia de CU 25.</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>CU 26</t>
+  </si>
+  <si>
+    <t>Realizar prototipo, descripción y diagramas de robustez y secuencia de CU 26.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,7 +401,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +447,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -566,18 +587,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -607,6 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -642,7 +652,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -978,14 +988,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AJ6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AG38" sqref="AG38"/>
+      <selection pane="bottomRight" activeCell="AL43" sqref="AL43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,84 +1070,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="35"/>
+      <c r="L4" s="32"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="35"/>
+      <c r="O4" s="32"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="34" t="s">
+      <c r="Q4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="35"/>
+      <c r="R4" s="32"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="34" t="s">
+      <c r="T4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="35"/>
+      <c r="U4" s="32"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="34" t="s">
+      <c r="W4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="35"/>
+      <c r="X4" s="32"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="34" t="s">
+      <c r="Z4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="35"/>
+      <c r="AA4" s="32"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="34" t="s">
+      <c r="AC4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="35"/>
+      <c r="AD4" s="32"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="34" t="s">
+      <c r="AF4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="35"/>
+      <c r="AG4" s="32"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="34" t="s">
+      <c r="AI4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="35"/>
+      <c r="AJ4" s="32"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="34" t="s">
+      <c r="AL4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="35"/>
+      <c r="AM4" s="32"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="34" t="s">
+      <c r="AO4" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="35"/>
+      <c r="AP4" s="32"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="34" t="s">
+      <c r="AR4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="35"/>
+      <c r="AS4" s="32"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="34" t="s">
+      <c r="AU4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="35"/>
+      <c r="AV4" s="32"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="34" t="s">
+      <c r="AX4" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="35"/>
-      <c r="AZ4" s="34" t="s">
+      <c r="AY4" s="32"/>
+      <c r="AZ4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="35"/>
+      <c r="BA4" s="32"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1270,14 +1280,14 @@
       </c>
     </row>
     <row r="6" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="17" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="24" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1387,12 +1397,12 @@
       </c>
     </row>
     <row r="7" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="25" t="s">
         <v>76</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1502,12 +1512,12 @@
       </c>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="26" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1617,12 +1627,12 @@
       </c>
     </row>
     <row r="9" spans="2:53" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1732,12 +1742,12 @@
       </c>
     </row>
     <row r="10" spans="2:53" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1847,12 +1857,12 @@
       </c>
     </row>
     <row r="11" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="26" t="s">
         <v>77</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1962,12 +1972,12 @@
       </c>
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="28" t="s">
         <v>78</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -2077,12 +2087,12 @@
       </c>
     </row>
     <row r="13" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -2192,12 +2202,12 @@
       </c>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="29" t="s">
         <v>77</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2307,14 +2317,14 @@
       </c>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="29" t="s">
         <v>77</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2424,12 +2434,12 @@
       </c>
     </row>
     <row r="16" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -2539,14 +2549,14 @@
       </c>
     </row>
     <row r="17" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="18" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -2656,14 +2666,14 @@
       </c>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -2773,14 +2783,14 @@
       </c>
     </row>
     <row r="19" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -2890,14 +2900,14 @@
       </c>
     </row>
     <row r="20" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -3007,14 +3017,14 @@
       </c>
     </row>
     <row r="21" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -3124,14 +3134,14 @@
       </c>
     </row>
     <row r="22" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -3241,14 +3251,14 @@
       </c>
     </row>
     <row r="23" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -3358,14 +3368,14 @@
       </c>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -3475,14 +3485,14 @@
       </c>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -3592,14 +3602,14 @@
       </c>
     </row>
     <row r="26" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -3709,14 +3719,14 @@
       </c>
     </row>
     <row r="27" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -3826,14 +3836,14 @@
       </c>
     </row>
     <row r="28" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -3943,14 +3953,14 @@
       </c>
     </row>
     <row r="29" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -4060,14 +4070,14 @@
       </c>
     </row>
     <row r="30" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -4177,14 +4187,14 @@
       </c>
     </row>
     <row r="31" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="18" t="s">
         <v>56</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -4294,14 +4304,14 @@
       </c>
     </row>
     <row r="32" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="18" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -4411,14 +4421,14 @@
       </c>
     </row>
     <row r="33" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="32" t="s">
+      <c r="E33" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="5" t="s">
@@ -4528,14 +4538,14 @@
       </c>
     </row>
     <row r="34" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="18" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -4645,14 +4655,14 @@
       </c>
     </row>
     <row r="35" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="18" t="s">
         <v>60</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -4762,14 +4772,14 @@
       </c>
     </row>
     <row r="36" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="18" t="s">
         <v>61</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -4879,14 +4889,14 @@
       </c>
     </row>
     <row r="37" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="32" t="s">
+      <c r="E37" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -4996,14 +5006,14 @@
       </c>
     </row>
     <row r="38" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="18" t="s">
         <v>63</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E38" s="32" t="s">
+      <c r="E38" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -5113,14 +5123,14 @@
       </c>
     </row>
     <row r="39" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="18" t="s">
         <v>64</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -5230,14 +5240,14 @@
       </c>
     </row>
     <row r="40" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C40" s="13"/>
-      <c r="D40" s="25" t="s">
+      <c r="D40" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -5337,122 +5347,248 @@
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="AZ40" s="16" t="e">
-        <f>H40+K40+N40+Q40+T40+W40+Z40+AC40+AF40+AI40+AL40+AO40+AR40+AU40+AX40+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+      <c r="AZ40" s="16">
+        <f>H40+K40+N40+Q40+T40+W40+Z40+AC40+AF40+AI40+AL40+AO40+AR40+AU40+AX40</f>
+        <v>1</v>
+      </c>
+      <c r="BA40" s="16">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:53" x14ac:dyDescent="0.25">
+      <c r="B41" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G41" s="13">
+        <v>1</v>
+      </c>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14">
+        <f t="shared" ref="I41" si="84">G41-H41</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="15"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14">
+        <f t="shared" ref="L41" si="85">I41-K41</f>
+        <v>1</v>
+      </c>
+      <c r="M41" s="15"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14">
+        <f t="shared" ref="O41" si="86">L41-N41</f>
+        <v>1</v>
+      </c>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14">
+        <f t="shared" ref="R41" si="87">O41-Q41</f>
+        <v>1</v>
+      </c>
+      <c r="S41" s="15"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14">
+        <f t="shared" ref="U41" si="88">R41-T41</f>
+        <v>1</v>
+      </c>
+      <c r="V41" s="15"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14">
+        <f t="shared" ref="X41" si="89">U41-W41</f>
+        <v>1</v>
+      </c>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="14"/>
+      <c r="AA41" s="14">
+        <f t="shared" ref="AA41" si="90">X41-Z41</f>
+        <v>1</v>
+      </c>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="14"/>
+      <c r="AD41" s="14">
+        <f t="shared" ref="AD41" si="91">AA41-AC41</f>
+        <v>1</v>
+      </c>
+      <c r="AE41" s="15"/>
+      <c r="AF41" s="14"/>
+      <c r="AG41" s="14">
+        <f t="shared" ref="AG41" si="92">AD41-AF41</f>
+        <v>1</v>
+      </c>
+      <c r="AH41" s="15"/>
+      <c r="AI41" s="14"/>
+      <c r="AJ41" s="14">
+        <f t="shared" ref="AJ41" si="93">AG41-AI41</f>
+        <v>1</v>
+      </c>
+      <c r="AK41" s="15"/>
+      <c r="AL41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AM41" s="14">
+        <f t="shared" ref="AM41" si="94">AJ41-AL41</f>
+        <v>0</v>
+      </c>
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="14"/>
+      <c r="AP41" s="14">
+        <f t="shared" ref="AP41" si="95">AM41-AO41</f>
+        <v>0</v>
+      </c>
+      <c r="AQ41" s="15"/>
+      <c r="AR41" s="14"/>
+      <c r="AS41" s="14">
+        <f t="shared" ref="AS41" si="96">AP41-AR41</f>
+        <v>0</v>
+      </c>
+      <c r="AT41" s="15"/>
+      <c r="AU41" s="14"/>
+      <c r="AV41" s="14">
+        <f t="shared" ref="AV41" si="97">AS41-AU41</f>
+        <v>0</v>
+      </c>
+      <c r="AW41" s="15"/>
+      <c r="AX41" s="14"/>
+      <c r="AY41" s="14">
+        <f t="shared" ref="AY41" si="98">AV41-AX41</f>
+        <v>0</v>
+      </c>
+      <c r="AZ41" s="16">
+        <f>H41+K41+N41+Q41+T41+W41+Z41+AC41+AF41+AI41+AL41+AO41+AR41+AU41+AX41</f>
+        <v>1</v>
+      </c>
+      <c r="BA41" s="16">
+        <f t="shared" ref="BA41" si="99">G41-AZ41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" s="13">
+        <v>1</v>
+      </c>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14">
+        <f t="shared" ref="I42" si="100">G42-H42</f>
+        <v>1</v>
+      </c>
+      <c r="J42" s="15"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14">
+        <f t="shared" ref="L42" si="101">I42-K42</f>
+        <v>1</v>
+      </c>
+      <c r="M42" s="15"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14">
+        <f t="shared" ref="O42" si="102">L42-N42</f>
+        <v>1</v>
+      </c>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14">
+        <f t="shared" ref="R42" si="103">O42-Q42</f>
+        <v>1</v>
+      </c>
+      <c r="S42" s="15"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14">
+        <f t="shared" ref="U42" si="104">R42-T42</f>
+        <v>1</v>
+      </c>
+      <c r="V42" s="15"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14">
+        <f t="shared" ref="X42" si="105">U42-W42</f>
+        <v>1</v>
+      </c>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14">
+        <f t="shared" ref="AA42" si="106">X42-Z42</f>
+        <v>1</v>
+      </c>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14">
+        <f t="shared" ref="AD42" si="107">AA42-AC42</f>
+        <v>1</v>
+      </c>
+      <c r="AE42" s="15"/>
+      <c r="AF42" s="14"/>
+      <c r="AG42" s="14">
+        <f t="shared" ref="AG42" si="108">AD42-AF42</f>
+        <v>1</v>
+      </c>
+      <c r="AH42" s="15"/>
+      <c r="AI42" s="14"/>
+      <c r="AJ42" s="14">
+        <f t="shared" ref="AJ42" si="109">AG42-AI42</f>
+        <v>1</v>
+      </c>
+      <c r="AK42" s="15"/>
+      <c r="AL42" s="14">
+        <v>2</v>
+      </c>
+      <c r="AM42" s="14">
+        <f t="shared" ref="AM42" si="110">AJ42-AL42</f>
+        <v>-1</v>
+      </c>
+      <c r="AN42" s="15"/>
+      <c r="AO42" s="14"/>
+      <c r="AP42" s="14">
+        <f t="shared" ref="AP42" si="111">AM42-AO42</f>
+        <v>-1</v>
+      </c>
+      <c r="AQ42" s="15"/>
+      <c r="AR42" s="14"/>
+      <c r="AS42" s="14">
+        <f t="shared" ref="AS42" si="112">AP42-AR42</f>
+        <v>-1</v>
+      </c>
+      <c r="AT42" s="15"/>
+      <c r="AU42" s="14"/>
+      <c r="AV42" s="14">
+        <f t="shared" ref="AV42" si="113">AS42-AU42</f>
+        <v>-1</v>
+      </c>
+      <c r="AW42" s="15"/>
+      <c r="AX42" s="14"/>
+      <c r="AY42" s="14">
+        <f t="shared" ref="AY42" si="114">AV42-AX42</f>
+        <v>-1</v>
+      </c>
+      <c r="AZ42" s="16" t="e">
+        <f>H42+K42+N42+Q42+T42+W42+Z42+AC42+AF42+AI42+AL42+AO42+AR42+AU42+AX42+#REF!+#REF!+#REF!+#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="BA40" s="16" t="e">
-        <f t="shared" si="49"/>
+      <c r="BA42" s="16" t="e">
+        <f t="shared" ref="BA42" si="115">G42-AZ42</f>
         <v>#REF!</v>
       </c>
-    </row>
-    <row r="41" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="18"/>
-      <c r="X41" s="18"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="18"/>
-      <c r="AA41" s="18"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="18"/>
-      <c r="AD41" s="18"/>
-      <c r="AE41" s="19"/>
-      <c r="AF41" s="18"/>
-      <c r="AG41" s="18"/>
-      <c r="AH41" s="19"/>
-      <c r="AI41" s="18"/>
-      <c r="AJ41" s="18"/>
-      <c r="AK41" s="19"/>
-      <c r="AL41" s="18"/>
-      <c r="AM41" s="18"/>
-      <c r="AN41" s="19"/>
-      <c r="AO41" s="18"/>
-      <c r="AP41" s="18"/>
-      <c r="AQ41" s="19"/>
-      <c r="AR41" s="18"/>
-      <c r="AS41" s="18"/>
-      <c r="AT41" s="19"/>
-      <c r="AU41" s="18"/>
-      <c r="AV41" s="18"/>
-      <c r="AW41" s="19"/>
-      <c r="AX41" s="18"/>
-      <c r="AY41" s="18"/>
-      <c r="AZ41" s="20"/>
-      <c r="BA41" s="20"/>
-    </row>
-    <row r="42" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="18"/>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="19"/>
-      <c r="Z42" s="18"/>
-      <c r="AA42" s="18"/>
-      <c r="AB42" s="19"/>
-      <c r="AC42" s="18"/>
-      <c r="AD42" s="18"/>
-      <c r="AE42" s="19"/>
-      <c r="AF42" s="18"/>
-      <c r="AG42" s="18"/>
-      <c r="AH42" s="19"/>
-      <c r="AI42" s="18"/>
-      <c r="AJ42" s="18"/>
-      <c r="AK42" s="19"/>
-      <c r="AL42" s="18"/>
-      <c r="AM42" s="18"/>
-      <c r="AN42" s="19"/>
-      <c r="AO42" s="18"/>
-      <c r="AP42" s="18"/>
-      <c r="AQ42" s="19"/>
-      <c r="AR42" s="18"/>
-      <c r="AS42" s="18"/>
-      <c r="AT42" s="19"/>
-      <c r="AU42" s="18"/>
-      <c r="AV42" s="18"/>
-      <c r="AW42" s="19"/>
-      <c r="AX42" s="18"/>
-      <c r="AY42" s="18"/>
-      <c r="AZ42" s="20"/>
-      <c r="BA42" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5489,7 +5625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>